<commit_message>
fixed the geopoint stuff
</commit_message>
<xml_diff>
--- a/Location Coordinates.xlsx
+++ b/Location Coordinates.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkn286/Documents/GitHub/Look-for-UT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xindixu/Files/Computer Science/iOS Development/Group15Alpha/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24980" yWindow="6180" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="11240" yWindow="460" windowWidth="17560" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Question Number</t>
   </si>
@@ -37,13 +37,16 @@
   <si>
     <t>Latitude</t>
   </si>
+  <si>
+    <t>little field fountain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -76,7 +79,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -379,8 +382,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>30.2837284764915</v>
@@ -391,156 +394,145 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>30.285441285189599</v>
+        <v>30.2837284764915</v>
       </c>
       <c r="C3" s="1">
-        <v>-97.735724821686702</v>
+        <v>-97.739589214324894</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>30.283015086901401</v>
+        <v>30.285441285189599</v>
       </c>
       <c r="C4" s="1">
-        <v>-97.737016975879598</v>
+        <v>-97.735724821686702</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>30.289724913146301</v>
+        <v>30.283015086901401</v>
       </c>
       <c r="C5" s="1">
-        <v>-97.738473415374699</v>
+        <v>-97.737016975879598</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>30.2862808863749</v>
+        <v>30.286693156878201</v>
       </c>
       <c r="C6" s="1">
-        <v>-97.736974060535402</v>
+        <v>-97.740957140922504</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>30.289081049140002</v>
+        <v>30.2862808863749</v>
       </c>
       <c r="C7" s="1">
-        <v>-97.740678191184898</v>
+        <v>-97.736974060535402</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>30.283865131697599</v>
+        <v>30.289081049140002</v>
       </c>
       <c r="C8" s="1">
-        <v>-97.7382239699363</v>
+        <v>-97.740678191184898</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>30.2867811694578</v>
+        <v>30.283865131697599</v>
       </c>
       <c r="C9" s="1">
-        <v>-97.740332186222005</v>
+        <v>-97.7382239699363</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>30.288407071857801</v>
+        <v>30.2867811694578</v>
       </c>
       <c r="C10" s="1">
-        <v>-97.736746072769094</v>
+        <v>-97.740332186222005</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>30.283450533112099</v>
+        <v>30.288407071857801</v>
       </c>
       <c r="C11" s="1">
-        <v>-97.738524377345996</v>
+        <v>-97.736746072769094</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>30.282357699999999</v>
+        <v>30.283450533112099</v>
       </c>
       <c r="C12" s="1">
-        <v>-97.745289499999998</v>
+        <v>-97.738524377345996</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>30.287693716288</v>
+        <v>30.2840434780362</v>
       </c>
       <c r="C13" s="1">
-        <v>-97.739219069480896</v>
+        <v>-97.736920416355105</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>30.286125705455699</v>
+        <v>30.287693716288</v>
       </c>
       <c r="C14" s="1">
-        <v>-97.737349569797502</v>
+        <v>-97.739219069480896</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>30.2840434780362</v>
+        <v>30.286125705455699</v>
       </c>
       <c r="C15" s="1">
-        <v>-97.736920416355105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>30.286693156878201</v>
-      </c>
-      <c r="C16" s="1">
-        <v>-97.740957140922504</v>
+        <v>-97.737349569797502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>